<commit_message>
Initializations for the type bateau
</commit_message>
<xml_diff>
--- a/dataFiles/init/bateau/bateau_1.xlsx
+++ b/dataFiles/init/bateau/bateau_1.xlsx
@@ -19,22 +19,22 @@
     <t>Bbox</t>
   </si>
   <si>
-    <t>(422, 500, 119, 189)</t>
-  </si>
-  <si>
-    <t>(631, 483, 92, 167)</t>
-  </si>
-  <si>
-    <t>(910, 487, 92, 147)</t>
-  </si>
-  <si>
-    <t>(1046, 485, 74, 128)</t>
-  </si>
-  <si>
-    <t>(1196, 475, 51, 119)</t>
-  </si>
-  <si>
-    <t>(1311, 475, 52, 101)</t>
+    <t>(419, 499, 117, 187)</t>
+  </si>
+  <si>
+    <t>(634, 489, 87, 157)</t>
+  </si>
+  <si>
+    <t>(912, 490, 89, 139)</t>
+  </si>
+  <si>
+    <t>(1047, 480, 73, 132)</t>
+  </si>
+  <si>
+    <t>(1196, 473, 47, 121)</t>
+  </si>
+  <si>
+    <t>(1310, 476, 46, 101)</t>
   </si>
 </sst>
 </file>

</xml_diff>